<commit_message>
Atualizando o cronograma 3 e adicionando o 4
</commit_message>
<xml_diff>
--- a/Cronogramas/CRONOGRAMA-03 - GRUPO-02.xlsx
+++ b/Cronogramas/CRONOGRAMA-03 - GRUPO-02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOGIMIRIM-CLODOVEUBA\Documents\GitHub\TCC\Cronogramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11203577-0C66-4FE6-A600-6477C16E58B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F5A1A8-8A85-4FFF-B533-0749FAD71EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRONOGRAMA-03" sheetId="4" r:id="rId1"/>
@@ -451,23 +451,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -779,25 +768,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F779B1-8D3E-4391-A788-FB6D40123DAC}">
   <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" customWidth="1"/>
+    <col min="3" max="3" width="60.81640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
@@ -809,7 +798,7 @@
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="2:9" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -818,7 +807,7 @@
       </c>
       <c r="D3" s="22"/>
     </row>
-    <row r="4" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -827,7 +816,7 @@
       </c>
       <c r="D4" s="23"/>
     </row>
-    <row r="5" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
       <c r="G5" s="15" t="s">
         <v>3</v>
@@ -837,7 +826,7 @@
       </c>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
@@ -860,7 +849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="19" t="s">
         <v>20</v>
       </c>
@@ -880,10 +869,9 @@
         <f>F7-E7</f>
         <v>6</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="20"/>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -898,7 +886,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="20"/>
       <c r="C9" s="4" t="s">
         <v>2</v>
@@ -913,7 +901,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="20"/>
       <c r="C10" s="4" t="s">
         <v>2</v>
@@ -928,7 +916,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="20"/>
       <c r="C11" s="5" t="s">
         <v>2</v>
@@ -943,7 +931,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="20"/>
       <c r="C12" s="3" t="s">
         <v>21</v>
@@ -961,10 +949,9 @@
         <f>F12-E12</f>
         <v>5</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="20"/>
       <c r="C13" s="4" t="s">
         <v>2</v>
@@ -979,7 +966,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="20"/>
       <c r="C14" s="4" t="s">
         <v>2</v>
@@ -994,7 +981,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="20"/>
       <c r="C15" s="4" t="s">
         <v>2</v>
@@ -1009,7 +996,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="20"/>
       <c r="C16" s="5" t="s">
         <v>2</v>
@@ -1024,7 +1011,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="20"/>
       <c r="C17" s="3" t="s">
         <v>24</v>
@@ -1042,10 +1029,10 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="H17" s="26"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="20"/>
       <c r="C18" s="4" t="s">
         <v>2</v>
@@ -1060,7 +1047,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="20"/>
       <c r="C19" s="4" t="s">
         <v>2</v>
@@ -1075,7 +1062,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="20"/>
       <c r="C20" s="4" t="s">
         <v>2</v>
@@ -1090,7 +1077,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="20"/>
       <c r="C21" s="5" t="s">
         <v>2</v>
@@ -1105,7 +1092,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="20"/>
       <c r="C22" s="3" t="s">
         <v>22</v>
@@ -1123,10 +1110,9 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="20"/>
       <c r="C23" s="4" t="s">
         <v>2</v>
@@ -1141,7 +1127,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="20"/>
       <c r="C24" s="4" t="s">
         <v>2</v>
@@ -1156,7 +1142,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="20"/>
       <c r="C25" s="4" t="s">
         <v>2</v>
@@ -1171,7 +1157,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="20"/>
       <c r="C26" s="5" t="s">
         <v>2</v>
@@ -1186,7 +1172,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="20"/>
       <c r="C27" s="3" t="s">
         <v>25</v>
@@ -1204,10 +1190,9 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="20"/>
       <c r="C28" s="4" t="s">
         <v>2</v>
@@ -1222,7 +1207,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="20"/>
       <c r="C29" s="4" t="s">
         <v>2</v>
@@ -1237,7 +1222,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="20"/>
       <c r="C30" s="4" t="s">
         <v>2</v>
@@ -1252,7 +1237,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="20"/>
       <c r="C31" s="5" t="s">
         <v>2</v>
@@ -1267,7 +1252,7 @@
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="20"/>
       <c r="C32" s="3" t="s">
         <v>2</v>
@@ -1282,7 +1267,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="20"/>
       <c r="C33" s="4" t="s">
         <v>2</v>
@@ -1297,7 +1282,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="20"/>
       <c r="C34" s="4" t="s">
         <v>2</v>
@@ -1312,7 +1297,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="20"/>
       <c r="C35" s="4" t="s">
         <v>2</v>
@@ -1327,7 +1312,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="20"/>
       <c r="C36" s="5" t="s">
         <v>2</v>

</xml_diff>